<commit_message>
updating to tower design near 0.49Hz nat freq
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_VolturnUS-S_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_VolturnUS-S_FineGrid_tabular.xlsx
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1721.471486294227</v>
+        <v>2071.061429947496</v>
       </c>
     </row>
     <row r="32">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>11553.0039250559</v>
+        <v>10496.2647569867</v>
       </c>
     </row>
     <row r="37">
@@ -22004,28 +22004,28 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>108.665</v>
+        <v>131.381</v>
       </c>
       <c r="E2" t="n">
-        <v>26338.38068668807</v>
+        <v>31771.18554937052</v>
       </c>
       <c r="F2" t="n">
-        <v>322152.3596815087</v>
+        <v>386841.5943930847</v>
       </c>
       <c r="G2" t="n">
-        <v>322152.3596815087</v>
+        <v>386841.5943930847</v>
       </c>
       <c r="H2" t="n">
-        <v>8260316914910.479</v>
+        <v>9919015240848.328</v>
       </c>
       <c r="I2" t="n">
-        <v>8260316914910.479</v>
+        <v>9919015240848.328</v>
       </c>
       <c r="J2" t="n">
-        <v>6550431313524.01</v>
+        <v>7865779085992.724</v>
       </c>
       <c r="K2" t="n">
-        <v>675343094530.4633</v>
+        <v>814645783317.1927</v>
       </c>
     </row>
     <row r="3">
@@ -22037,28 +22037,28 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>108.665</v>
+        <v>131.381</v>
       </c>
       <c r="E3" t="n">
-        <v>26338.38068668807</v>
+        <v>31771.18554937052</v>
       </c>
       <c r="F3" t="n">
-        <v>322152.3596815087</v>
+        <v>386841.5943930847</v>
       </c>
       <c r="G3" t="n">
-        <v>322152.3596815087</v>
+        <v>386841.5943930847</v>
       </c>
       <c r="H3" t="n">
-        <v>8260316914910.479</v>
+        <v>9919015240848.328</v>
       </c>
       <c r="I3" t="n">
-        <v>8260316914910.479</v>
+        <v>9919015240848.328</v>
       </c>
       <c r="J3" t="n">
-        <v>6550431313524.01</v>
+        <v>7865779085992.724</v>
       </c>
       <c r="K3" t="n">
-        <v>675343094530.4633</v>
+        <v>814645783317.1927</v>
       </c>
     </row>
     <row r="4">
@@ -22070,28 +22070,28 @@
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>102.037</v>
+        <v>123.731</v>
       </c>
       <c r="E4" t="n">
-        <v>24748.44878167958</v>
+        <v>29944.42021094096</v>
       </c>
       <c r="F4" t="n">
-        <v>303106.8835242288</v>
+        <v>365157.2274739144</v>
       </c>
       <c r="G4" t="n">
-        <v>303106.8835242288</v>
+        <v>365157.2274739144</v>
       </c>
       <c r="H4" t="n">
-        <v>7771971372416.122</v>
+        <v>9363005832664.475</v>
       </c>
       <c r="I4" t="n">
-        <v>7771971372416.122</v>
+        <v>9363005832664.475</v>
       </c>
       <c r="J4" t="n">
-        <v>6163173298325.985</v>
+        <v>7424863625302.928</v>
       </c>
       <c r="K4" t="n">
-        <v>634575609786.656</v>
+        <v>767805646434.3838</v>
       </c>
     </row>
     <row r="5">
@@ -22103,28 +22103,28 @@
         <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>102.037</v>
+        <v>123.731</v>
       </c>
       <c r="E5" t="n">
-        <v>24748.44878167958</v>
+        <v>29944.42021094096</v>
       </c>
       <c r="F5" t="n">
-        <v>303106.8835242288</v>
+        <v>365157.2274739144</v>
       </c>
       <c r="G5" t="n">
-        <v>303106.8835242288</v>
+        <v>365157.2274739144</v>
       </c>
       <c r="H5" t="n">
-        <v>7771971372416.122</v>
+        <v>9363005832664.475</v>
       </c>
       <c r="I5" t="n">
-        <v>7771971372416.122</v>
+        <v>9363005832664.475</v>
       </c>
       <c r="J5" t="n">
-        <v>6163173298325.985</v>
+        <v>7424863625302.928</v>
       </c>
       <c r="K5" t="n">
-        <v>634575609786.656</v>
+        <v>767805646434.3838</v>
       </c>
     </row>
     <row r="6">
@@ -22136,28 +22136,28 @@
         <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>95.36</v>
+        <v>116.046</v>
       </c>
       <c r="E6" t="n">
-        <v>23144.58579167808</v>
+        <v>28106.40928924677</v>
       </c>
       <c r="F6" t="n">
-        <v>283842.2696372339</v>
+        <v>343270.6501482529</v>
       </c>
       <c r="G6" t="n">
-        <v>283842.2696372339</v>
+        <v>343270.6501482529</v>
       </c>
       <c r="H6" t="n">
-        <v>7278006913775.228</v>
+        <v>8801811542262.895</v>
       </c>
       <c r="I6" t="n">
-        <v>7278006913775.228</v>
+        <v>8801811542262.895</v>
       </c>
       <c r="J6" t="n">
-        <v>5771459482623.756</v>
+        <v>6979836553014.476</v>
       </c>
       <c r="K6" t="n">
-        <v>593450917735.3356</v>
+        <v>720677161262.7379</v>
       </c>
     </row>
     <row r="7">
@@ -22169,28 +22169,28 @@
         <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>95.36</v>
+        <v>116.046</v>
       </c>
       <c r="E7" t="n">
-        <v>23144.58579167808</v>
+        <v>28106.40928924677</v>
       </c>
       <c r="F7" t="n">
-        <v>283842.2696372339</v>
+        <v>343270.6501482529</v>
       </c>
       <c r="G7" t="n">
-        <v>283842.2696372339</v>
+        <v>343270.6501482529</v>
       </c>
       <c r="H7" t="n">
-        <v>7278006913775.228</v>
+        <v>8801811542262.895</v>
       </c>
       <c r="I7" t="n">
-        <v>7278006913775.228</v>
+        <v>8801811542262.895</v>
       </c>
       <c r="J7" t="n">
-        <v>5771459482623.756</v>
+        <v>6979836553014.476</v>
       </c>
       <c r="K7" t="n">
-        <v>593450917735.3356</v>
+        <v>720677161262.7379</v>
       </c>
     </row>
     <row r="8">
@@ -22202,28 +22202,28 @@
         <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>88.229</v>
+        <v>107.964</v>
       </c>
       <c r="E8" t="n">
-        <v>21429.25594155661</v>
+        <v>26170.32584995283</v>
       </c>
       <c r="F8" t="n">
-        <v>263180.6979549173</v>
+        <v>320141.7022777938</v>
       </c>
       <c r="G8" t="n">
-        <v>263180.6979549173</v>
+        <v>320141.7022777938</v>
       </c>
       <c r="H8" t="n">
-        <v>6748223024485.059</v>
+        <v>8208761596866.509</v>
       </c>
       <c r="I8" t="n">
-        <v>6748223024485.059</v>
+        <v>8208761596866.509</v>
       </c>
       <c r="J8" t="n">
-        <v>5351340858416.651</v>
+        <v>6509547946315.142</v>
       </c>
       <c r="K8" t="n">
-        <v>549468101065.5542</v>
+        <v>671033996152.637</v>
       </c>
     </row>
     <row r="9">
@@ -22235,28 +22235,28 @@
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>88.229</v>
+        <v>107.964</v>
       </c>
       <c r="E9" t="n">
-        <v>21429.25594155661</v>
+        <v>26170.32584995283</v>
       </c>
       <c r="F9" t="n">
-        <v>263180.6979549173</v>
+        <v>320141.7022777938</v>
       </c>
       <c r="G9" t="n">
-        <v>263180.6979549173</v>
+        <v>320141.7022777938</v>
       </c>
       <c r="H9" t="n">
-        <v>6748223024485.059</v>
+        <v>8208761596866.509</v>
       </c>
       <c r="I9" t="n">
-        <v>6748223024485.059</v>
+        <v>8208761596866.509</v>
       </c>
       <c r="J9" t="n">
-        <v>5351340858416.651</v>
+        <v>6509547946315.142</v>
       </c>
       <c r="K9" t="n">
-        <v>549468101065.5542</v>
+        <v>671033996152.637</v>
       </c>
     </row>
     <row r="10">
@@ -22268,28 +22268,28 @@
         <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>81.086</v>
+        <v>99.861</v>
       </c>
       <c r="E10" t="n">
-        <v>19708.54109472723</v>
+        <v>24225.99807297111</v>
       </c>
       <c r="F10" t="n">
-        <v>242393.9423918938</v>
+        <v>296837.2916697407</v>
       </c>
       <c r="G10" t="n">
-        <v>242393.9423918938</v>
+        <v>296837.2916697407</v>
       </c>
       <c r="H10" t="n">
-        <v>6215229292099.843</v>
+        <v>7611212606916.429</v>
       </c>
       <c r="I10" t="n">
-        <v>6215229292099.843</v>
+        <v>7611212606916.429</v>
       </c>
       <c r="J10" t="n">
-        <v>4928676828635.175</v>
+        <v>6035691597284.729</v>
       </c>
       <c r="K10" t="n">
-        <v>505347207557.1086</v>
+        <v>621179437768.4901</v>
       </c>
     </row>
     <row r="11">
@@ -22301,28 +22301,28 @@
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>81.086</v>
+        <v>99.861</v>
       </c>
       <c r="E11" t="n">
-        <v>19708.54109472723</v>
+        <v>24225.99807297111</v>
       </c>
       <c r="F11" t="n">
-        <v>242393.9423918938</v>
+        <v>296837.2916697407</v>
       </c>
       <c r="G11" t="n">
-        <v>242393.9423918938</v>
+        <v>296837.2916697407</v>
       </c>
       <c r="H11" t="n">
-        <v>6215229292099.843</v>
+        <v>7611212606916.429</v>
       </c>
       <c r="I11" t="n">
-        <v>6215229292099.843</v>
+        <v>7611212606916.429</v>
       </c>
       <c r="J11" t="n">
-        <v>4928676828635.175</v>
+        <v>6035691597284.729</v>
       </c>
       <c r="K11" t="n">
-        <v>505347207557.1086</v>
+        <v>621179437768.4901</v>
       </c>
     </row>
     <row r="12">
@@ -22334,28 +22334,28 @@
         <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>74.217</v>
+        <v>91.105</v>
       </c>
       <c r="E12" t="n">
-        <v>18051.47303715258</v>
+        <v>22121.36462497203</v>
       </c>
       <c r="F12" t="n">
-        <v>222318.9551427827</v>
+        <v>271524.5430026618</v>
       </c>
       <c r="G12" t="n">
-        <v>222318.9551427827</v>
+        <v>271524.5430026618</v>
       </c>
       <c r="H12" t="n">
-        <v>5700486029302.119</v>
+        <v>6962167769299.023</v>
       </c>
       <c r="I12" t="n">
-        <v>5700486029302.119</v>
+        <v>6962167769299.023</v>
       </c>
       <c r="J12" t="n">
-        <v>4520485421236.581</v>
+        <v>5520999041054.125</v>
       </c>
       <c r="K12" t="n">
-        <v>462858283003.9124</v>
+        <v>567214477563.3855</v>
       </c>
     </row>
     <row r="13">
@@ -22367,28 +22367,28 @@
         <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>74.217</v>
+        <v>91.105</v>
       </c>
       <c r="E13" t="n">
-        <v>18051.47303715258</v>
+        <v>22121.36462497203</v>
       </c>
       <c r="F13" t="n">
-        <v>222318.9551427827</v>
+        <v>271524.5430026618</v>
       </c>
       <c r="G13" t="n">
-        <v>222318.9551427827</v>
+        <v>271524.5430026618</v>
       </c>
       <c r="H13" t="n">
-        <v>5700486029302.119</v>
+        <v>6962167769299.023</v>
       </c>
       <c r="I13" t="n">
-        <v>5700486029302.119</v>
+        <v>6962167769299.023</v>
       </c>
       <c r="J13" t="n">
-        <v>4520485421236.581</v>
+        <v>5520999041054.125</v>
       </c>
       <c r="K13" t="n">
-        <v>462858283003.9124</v>
+        <v>567214477563.3855</v>
       </c>
     </row>
     <row r="14">
@@ -22400,28 +22400,28 @@
         <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>67.36799999999999</v>
+        <v>82.36199999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>16396.92744911857</v>
+        <v>20016.10689458135</v>
       </c>
       <c r="F14" t="n">
-        <v>202218.6267412874</v>
+        <v>246113.8645026345</v>
       </c>
       <c r="G14" t="n">
-        <v>202218.6267412874</v>
+        <v>246113.8645026345</v>
       </c>
       <c r="H14" t="n">
-        <v>5185092993366.345</v>
+        <v>6310611910323.963</v>
       </c>
       <c r="I14" t="n">
-        <v>5185092993366.345</v>
+        <v>6310611910323.963</v>
       </c>
       <c r="J14" t="n">
-        <v>4111778743739.511</v>
+        <v>5004315244886.902</v>
       </c>
       <c r="K14" t="n">
-        <v>420434037156.8865</v>
+        <v>513233510117.4705</v>
       </c>
     </row>
     <row r="15">
@@ -22433,28 +22433,28 @@
         <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>67.36799999999999</v>
+        <v>82.36199999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>16396.92744911857</v>
+        <v>20016.10689458135</v>
       </c>
       <c r="F15" t="n">
-        <v>202218.6267412874</v>
+        <v>246113.8645026345</v>
       </c>
       <c r="G15" t="n">
-        <v>202218.6267412874</v>
+        <v>246113.8645026345</v>
       </c>
       <c r="H15" t="n">
-        <v>5185092993366.345</v>
+        <v>6310611910323.963</v>
       </c>
       <c r="I15" t="n">
-        <v>5185092993366.345</v>
+        <v>6310611910323.963</v>
       </c>
       <c r="J15" t="n">
-        <v>4111778743739.511</v>
+        <v>5004315244886.902</v>
       </c>
       <c r="K15" t="n">
-        <v>420434037156.8865</v>
+        <v>513233510117.4705</v>
       </c>
     </row>
     <row r="16">
@@ -22466,28 +22466,28 @@
         <v>10</v>
       </c>
       <c r="D16" t="n">
-        <v>60.325</v>
+        <v>73.57299999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>14693.118810091</v>
+        <v>17895.99680653546</v>
       </c>
       <c r="F16" t="n">
-        <v>181461.4465984184</v>
+        <v>220432.5223455892</v>
       </c>
       <c r="G16" t="n">
-        <v>181461.4465984184</v>
+        <v>220432.5223455892</v>
       </c>
       <c r="H16" t="n">
-        <v>4652857605087.651</v>
+        <v>5652115957579.212</v>
       </c>
       <c r="I16" t="n">
-        <v>4652857605087.651</v>
+        <v>5652115957579.212</v>
       </c>
       <c r="J16" t="n">
-        <v>3689716080834.508</v>
+        <v>4482127954360.315</v>
       </c>
       <c r="K16" t="n">
-        <v>376746636156.1794</v>
+        <v>458871712988.0887</v>
       </c>
     </row>
     <row r="17">
@@ -22499,28 +22499,28 @@
         <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>60.325</v>
+        <v>73.57299999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>14693.118810091</v>
+        <v>17895.99680653546</v>
       </c>
       <c r="F17" t="n">
-        <v>181461.4465984184</v>
+        <v>220432.5223455892</v>
       </c>
       <c r="G17" t="n">
-        <v>181461.4465984184</v>
+        <v>220432.5223455892</v>
       </c>
       <c r="H17" t="n">
-        <v>4652857605087.651</v>
+        <v>5652115957579.212</v>
       </c>
       <c r="I17" t="n">
-        <v>4652857605087.651</v>
+        <v>5652115957579.212</v>
       </c>
       <c r="J17" t="n">
-        <v>3689716080834.508</v>
+        <v>4482127954360.315</v>
       </c>
       <c r="K17" t="n">
-        <v>376746636156.1794</v>
+        <v>458871712988.0887</v>
       </c>
     </row>
     <row r="18">
@@ -22532,28 +22532,28 @@
         <v>10</v>
       </c>
       <c r="D18" t="n">
-        <v>53.288</v>
+        <v>64.80500000000001</v>
       </c>
       <c r="E18" t="n">
-        <v>12988.33374044083</v>
+        <v>15777.18019887476</v>
       </c>
       <c r="F18" t="n">
-        <v>160633.0863882673</v>
+        <v>194675.2168876515</v>
       </c>
       <c r="G18" t="n">
-        <v>160633.0863882673</v>
+        <v>194675.2168876515</v>
       </c>
       <c r="H18" t="n">
-        <v>4118797086878.649</v>
+        <v>4991672227888.5</v>
       </c>
       <c r="I18" t="n">
-        <v>4118797086878.649</v>
+        <v>4991672227888.5</v>
       </c>
       <c r="J18" t="n">
-        <v>3266206089894.769</v>
+        <v>3958396076715.581</v>
       </c>
       <c r="K18" t="n">
-        <v>333034198472.8419</v>
+        <v>404543082022.4297</v>
       </c>
     </row>
     <row r="19">
@@ -22565,28 +22565,28 @@
         <v>10</v>
       </c>
       <c r="D19" t="n">
-        <v>53.288</v>
+        <v>64.80500000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>12988.33374044083</v>
+        <v>15777.18019887476</v>
       </c>
       <c r="F19" t="n">
-        <v>160633.0863882673</v>
+        <v>194675.2168876515</v>
       </c>
       <c r="G19" t="n">
-        <v>160633.0863882673</v>
+        <v>194675.2168876515</v>
       </c>
       <c r="H19" t="n">
-        <v>4118797086878.649</v>
+        <v>4991672227888.5</v>
       </c>
       <c r="I19" t="n">
-        <v>4118797086878.649</v>
+        <v>4991672227888.5</v>
       </c>
       <c r="J19" t="n">
-        <v>3266206089894.769</v>
+        <v>3958396076715.581</v>
       </c>
       <c r="K19" t="n">
-        <v>333034198472.8419</v>
+        <v>404543082022.4297</v>
       </c>
     </row>
     <row r="20">
@@ -22598,28 +22598,28 @@
         <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>46.612</v>
+        <v>56.218</v>
       </c>
       <c r="E20" t="n">
-        <v>11368.76127456282</v>
+        <v>13698.45101824825</v>
       </c>
       <c r="F20" t="n">
-        <v>140790.8893466336</v>
+        <v>169316.2122934376</v>
       </c>
       <c r="G20" t="n">
-        <v>140790.8893466336</v>
+        <v>169316.2122934376</v>
       </c>
       <c r="H20" t="n">
-        <v>3610022803759.835</v>
+        <v>4341441340857.376</v>
       </c>
       <c r="I20" t="n">
-        <v>3610022803759.835</v>
+        <v>4341441340857.376</v>
       </c>
       <c r="J20" t="n">
-        <v>2862748083381.55</v>
+        <v>3442762983299.899</v>
       </c>
       <c r="K20" t="n">
-        <v>291506699347.7645</v>
+        <v>351242333801.2372</v>
       </c>
     </row>
     <row r="21">
@@ -22631,28 +22631,28 @@
         <v>10</v>
       </c>
       <c r="D21" t="n">
-        <v>46.612</v>
+        <v>56.218</v>
       </c>
       <c r="E21" t="n">
-        <v>11368.76127456282</v>
+        <v>13698.45101824825</v>
       </c>
       <c r="F21" t="n">
-        <v>140790.8893466336</v>
+        <v>169316.2122934376</v>
       </c>
       <c r="G21" t="n">
-        <v>140790.8893466336</v>
+        <v>169316.2122934376</v>
       </c>
       <c r="H21" t="n">
-        <v>3610022803759.835</v>
+        <v>4341441340857.376</v>
       </c>
       <c r="I21" t="n">
-        <v>3610022803759.835</v>
+        <v>4341441340857.376</v>
       </c>
       <c r="J21" t="n">
-        <v>2862748083381.55</v>
+        <v>3442762983299.899</v>
       </c>
       <c r="K21" t="n">
-        <v>291506699347.7645</v>
+        <v>351242333801.2372</v>
       </c>
     </row>
     <row r="22">
@@ -22664,28 +22664,28 @@
         <v>10</v>
       </c>
       <c r="D22" t="n">
-        <v>39.958</v>
+        <v>47.635</v>
       </c>
       <c r="E22" t="n">
-        <v>9752.352436984766</v>
+        <v>11617.07893266584</v>
       </c>
       <c r="F22" t="n">
-        <v>120934.086968916</v>
+        <v>143836.6278297039</v>
       </c>
       <c r="G22" t="n">
-        <v>120934.086968916</v>
+        <v>143836.6278297039</v>
       </c>
       <c r="H22" t="n">
-        <v>3100874024844.001</v>
+        <v>3688118662300.099</v>
       </c>
       <c r="I22" t="n">
-        <v>3100874024844.001</v>
+        <v>3688118662300.099</v>
       </c>
       <c r="J22" t="n">
-        <v>2458993101701.293</v>
+        <v>2924678099203.979</v>
       </c>
       <c r="K22" t="n">
-        <v>250060318897.0453</v>
+        <v>297873818786.3037</v>
       </c>
     </row>
     <row r="23">
@@ -22697,28 +22697,28 @@
         <v>10</v>
       </c>
       <c r="D23" t="n">
-        <v>39.958</v>
+        <v>47.635</v>
       </c>
       <c r="E23" t="n">
-        <v>9752.352436984766</v>
+        <v>11617.07893266584</v>
       </c>
       <c r="F23" t="n">
-        <v>120934.086968916</v>
+        <v>143836.6278297039</v>
       </c>
       <c r="G23" t="n">
-        <v>120934.086968916</v>
+        <v>143836.6278297039</v>
       </c>
       <c r="H23" t="n">
-        <v>3100874024844.001</v>
+        <v>3688118662300.099</v>
       </c>
       <c r="I23" t="n">
-        <v>3100874024844.001</v>
+        <v>3688118662300.099</v>
       </c>
       <c r="J23" t="n">
-        <v>2458993101701.293</v>
+        <v>2924678099203.979</v>
       </c>
       <c r="K23" t="n">
-        <v>250060318897.0453</v>
+        <v>297873818786.3037</v>
       </c>
     </row>
     <row r="24">
@@ -22730,28 +22730,28 @@
         <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>33.68</v>
+        <v>40.136</v>
       </c>
       <c r="E24" t="n">
-        <v>8225.29315903275</v>
+        <v>9795.620956399958</v>
       </c>
       <c r="F24" t="n">
-        <v>102125.9273786147</v>
+        <v>121466.3142860007</v>
       </c>
       <c r="G24" t="n">
-        <v>102125.9273786147</v>
+        <v>121466.3142860007</v>
       </c>
       <c r="H24" t="n">
-        <v>2618613522528.582</v>
+        <v>3114520879128.223</v>
       </c>
       <c r="I24" t="n">
-        <v>2618613522528.582</v>
+        <v>3114520879128.223</v>
       </c>
       <c r="J24" t="n">
-        <v>2076560523365.165</v>
+        <v>2469815057148.681</v>
       </c>
       <c r="K24" t="n">
-        <v>210904952795.7115</v>
+        <v>251169768112.8195</v>
       </c>
     </row>
     <row r="25">
@@ -22763,28 +22763,28 @@
         <v>10</v>
       </c>
       <c r="D25" t="n">
-        <v>33.68</v>
+        <v>40.136</v>
       </c>
       <c r="E25" t="n">
-        <v>8225.29315903275</v>
+        <v>9795.620956399958</v>
       </c>
       <c r="F25" t="n">
-        <v>102125.9273786147</v>
+        <v>121466.3142860007</v>
       </c>
       <c r="G25" t="n">
-        <v>102125.9273786147</v>
+        <v>121466.3142860007</v>
       </c>
       <c r="H25" t="n">
-        <v>2618613522528.582</v>
+        <v>3114520879128.223</v>
       </c>
       <c r="I25" t="n">
-        <v>2618613522528.582</v>
+        <v>3114520879128.223</v>
       </c>
       <c r="J25" t="n">
-        <v>2076560523365.165</v>
+        <v>2469815057148.681</v>
       </c>
       <c r="K25" t="n">
-        <v>210904952795.7115</v>
+        <v>251169768112.8195</v>
       </c>
     </row>
     <row r="26">
@@ -22796,28 +22796,28 @@
         <v>10</v>
       </c>
       <c r="D26" t="n">
-        <v>27.365</v>
+        <v>32.598</v>
       </c>
       <c r="E26" t="n">
-        <v>6687.285300387766</v>
+        <v>7961.912586106368</v>
       </c>
       <c r="F26" t="n">
-        <v>83134.82428130708</v>
+        <v>98877.16640112977</v>
       </c>
       <c r="G26" t="n">
-        <v>83134.82428130708</v>
+        <v>98877.16640112977</v>
       </c>
       <c r="H26" t="n">
-        <v>2131662161059.156</v>
+        <v>2535311959003.328</v>
       </c>
       <c r="I26" t="n">
-        <v>2131662161059.156</v>
+        <v>2535311959003.328</v>
       </c>
       <c r="J26" t="n">
-        <v>1690408093719.911</v>
+        <v>2010502383489.639</v>
       </c>
       <c r="K26" t="n">
-        <v>171468853856.0966</v>
+        <v>204151604771.9582</v>
       </c>
     </row>
     <row r="27">
@@ -22829,28 +22829,28 @@
         <v>10</v>
       </c>
       <c r="D27" t="n">
-        <v>27.365</v>
+        <v>32.598</v>
       </c>
       <c r="E27" t="n">
-        <v>6687.285300387766</v>
+        <v>7961.912586106368</v>
       </c>
       <c r="F27" t="n">
-        <v>83134.82428130708</v>
+        <v>98877.16640112977</v>
       </c>
       <c r="G27" t="n">
-        <v>83134.82428130708</v>
+        <v>98877.16640112977</v>
       </c>
       <c r="H27" t="n">
-        <v>2131662161059.156</v>
+        <v>2535311959003.328</v>
       </c>
       <c r="I27" t="n">
-        <v>2131662161059.156</v>
+        <v>2535311959003.328</v>
       </c>
       <c r="J27" t="n">
-        <v>1690408093719.911</v>
+        <v>2010502383489.639</v>
       </c>
       <c r="K27" t="n">
-        <v>171468853856.0966</v>
+        <v>204151604771.9582</v>
       </c>
     </row>
     <row r="28">
@@ -22859,31 +22859,31 @@
         <v>105.863</v>
       </c>
       <c r="C28" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D28" t="n">
-        <v>21.89</v>
+        <v>25.661</v>
       </c>
       <c r="E28" t="n">
-        <v>5350.130685657279</v>
+        <v>6271.944066680704</v>
       </c>
       <c r="F28" t="n">
-        <v>66531.11508504837</v>
+        <v>77997.9724400553</v>
       </c>
       <c r="G28" t="n">
-        <v>66531.11508504837</v>
+        <v>77997.9724400553</v>
       </c>
       <c r="H28" t="n">
-        <v>1705926027821.753</v>
+        <v>1999948011283.469</v>
       </c>
       <c r="I28" t="n">
-        <v>1705926027821.753</v>
+        <v>1999948011283.469</v>
       </c>
       <c r="J28" t="n">
-        <v>1352799340062.65</v>
+        <v>1585958772947.791</v>
       </c>
       <c r="K28" t="n">
-        <v>137182838093.7764</v>
+        <v>160819078632.8386</v>
       </c>
     </row>
     <row r="29">
@@ -22895,28 +22895,28 @@
         <v>10</v>
       </c>
       <c r="D29" t="n">
-        <v>21.89</v>
+        <v>25.661</v>
       </c>
       <c r="E29" t="n">
-        <v>5352.276292908822</v>
+        <v>6271.944066680704</v>
       </c>
       <c r="F29" t="n">
-        <v>66611.19150659816</v>
+        <v>77997.9724400553</v>
       </c>
       <c r="G29" t="n">
-        <v>66611.19150659816</v>
+        <v>77997.9724400553</v>
       </c>
       <c r="H29" t="n">
-        <v>1707979269399.953</v>
+        <v>1999948011283.469</v>
       </c>
       <c r="I29" t="n">
-        <v>1707979269399.953</v>
+        <v>1999948011283.469</v>
       </c>
       <c r="J29" t="n">
-        <v>1354427560634.162</v>
+        <v>1585958772947.791</v>
       </c>
       <c r="K29" t="n">
-        <v>137237853664.3288</v>
+        <v>160819078632.8386</v>
       </c>
     </row>
     <row r="30">
@@ -22925,31 +22925,31 @@
         <v>105.864</v>
       </c>
       <c r="C30" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
-        <v>16.456</v>
+        <v>18.755</v>
       </c>
       <c r="E30" t="n">
-        <v>4024.199023964874</v>
+        <v>4587.18504571328</v>
       </c>
       <c r="F30" t="n">
-        <v>50097.0369703021</v>
+        <v>57125.13481819846</v>
       </c>
       <c r="G30" t="n">
-        <v>50097.0369703021</v>
+        <v>57125.13481819846</v>
       </c>
       <c r="H30" t="n">
-        <v>1284539409494.926</v>
+        <v>1464747046620.473</v>
       </c>
       <c r="I30" t="n">
-        <v>1284539409494.926</v>
+        <v>1464747046620.473</v>
       </c>
       <c r="J30" t="n">
-        <v>1018639751729.476</v>
+        <v>1161544407970.035</v>
       </c>
       <c r="K30" t="n">
-        <v>103184590358.0737</v>
+        <v>117620129377.2636</v>
       </c>
     </row>
     <row r="31">
@@ -22958,31 +22958,31 @@
         <v>118.843</v>
       </c>
       <c r="C31" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D31" t="n">
-        <v>16.456</v>
+        <v>18.755</v>
       </c>
       <c r="E31" t="n">
-        <v>4024.199023964874</v>
+        <v>4587.18504571328</v>
       </c>
       <c r="F31" t="n">
-        <v>50097.0369703021</v>
+        <v>57125.13481819846</v>
       </c>
       <c r="G31" t="n">
-        <v>50097.0369703021</v>
+        <v>57125.13481819846</v>
       </c>
       <c r="H31" t="n">
-        <v>1284539409494.926</v>
+        <v>1464747046620.473</v>
       </c>
       <c r="I31" t="n">
-        <v>1284539409494.926</v>
+        <v>1464747046620.473</v>
       </c>
       <c r="J31" t="n">
-        <v>1018639751729.476</v>
+        <v>1161544407970.035</v>
       </c>
       <c r="K31" t="n">
-        <v>103184590358.0737</v>
+        <v>117620129377.2636</v>
       </c>
     </row>
     <row r="32">
@@ -22991,31 +22991,31 @@
         <v>118.844</v>
       </c>
       <c r="C32" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>16.669</v>
+        <v>18.397</v>
       </c>
       <c r="E32" t="n">
-        <v>4076.199672526166</v>
+        <v>4499.785131470276</v>
       </c>
       <c r="F32" t="n">
-        <v>50742.22772625707</v>
+        <v>56040.73851334897</v>
       </c>
       <c r="G32" t="n">
-        <v>50742.22772625707</v>
+        <v>56040.73851334897</v>
       </c>
       <c r="H32" t="n">
-        <v>1301082762211.72</v>
+        <v>1436942013162.794</v>
       </c>
       <c r="I32" t="n">
-        <v>1301082762211.72</v>
+        <v>1436942013162.794</v>
       </c>
       <c r="J32" t="n">
-        <v>1031758630433.894</v>
+        <v>1139495016438.096</v>
       </c>
       <c r="K32" t="n">
-        <v>104517940321.1837</v>
+        <v>115379105935.1353</v>
       </c>
     </row>
     <row r="33">
@@ -23024,31 +23024,31 @@
         <v>118.844</v>
       </c>
       <c r="C33" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D33" t="n">
-        <v>16.669</v>
+        <v>18.397</v>
       </c>
       <c r="E33" t="n">
-        <v>4076.199672526166</v>
+        <v>4499.785131470276</v>
       </c>
       <c r="F33" t="n">
-        <v>50742.22772625707</v>
+        <v>56040.73851334897</v>
       </c>
       <c r="G33" t="n">
-        <v>50742.22772625707</v>
+        <v>56040.73851334897</v>
       </c>
       <c r="H33" t="n">
-        <v>1301082762211.72</v>
+        <v>1436942013162.794</v>
       </c>
       <c r="I33" t="n">
-        <v>1301082762211.72</v>
+        <v>1436942013162.794</v>
       </c>
       <c r="J33" t="n">
-        <v>1031758630433.894</v>
+        <v>1139495016438.096</v>
       </c>
       <c r="K33" t="n">
-        <v>104517940321.1837</v>
+        <v>115379105935.1353</v>
       </c>
     </row>
     <row r="34">
@@ -23057,31 +23057,31 @@
         <v>118.845</v>
       </c>
       <c r="C34" t="n">
-        <v>9.996</v>
+        <v>10</v>
       </c>
       <c r="D34" t="n">
-        <v>17.024</v>
+        <v>17.639</v>
       </c>
       <c r="E34" t="n">
-        <v>4162.862479056349</v>
+        <v>4314.710952782626</v>
       </c>
       <c r="F34" t="n">
-        <v>51817.36174723865</v>
+        <v>53743.95455720842</v>
       </c>
       <c r="G34" t="n">
-        <v>51817.36174723865</v>
+        <v>53743.95455720842</v>
       </c>
       <c r="H34" t="n">
-        <v>1328650301211.248</v>
+        <v>1378050116851.498</v>
       </c>
       <c r="I34" t="n">
-        <v>1328650301211.248</v>
+        <v>1378050116851.498</v>
       </c>
       <c r="J34" t="n">
-        <v>1053619688860.519</v>
+        <v>1092793742663.238</v>
       </c>
       <c r="K34" t="n">
-        <v>106740063565.5474</v>
+        <v>110633614173.9135</v>
       </c>
     </row>
     <row r="35">
@@ -23090,31 +23090,31 @@
         <v>131.823</v>
       </c>
       <c r="C35" t="n">
-        <v>9.992000000000001</v>
+        <v>9.994</v>
       </c>
       <c r="D35" t="n">
-        <v>17.024</v>
+        <v>17.639</v>
       </c>
       <c r="E35" t="n">
-        <v>4161.193825888314</v>
+        <v>4312.117551710823</v>
       </c>
       <c r="F35" t="n">
-        <v>51755.07500347148</v>
+        <v>53647.10293800638</v>
       </c>
       <c r="G35" t="n">
-        <v>51755.07500347148</v>
+        <v>53647.10293800638</v>
       </c>
       <c r="H35" t="n">
-        <v>1327053205217.217</v>
+        <v>1375566742000.164</v>
       </c>
       <c r="I35" t="n">
-        <v>1327053205217.217</v>
+        <v>1375566742000.164</v>
       </c>
       <c r="J35" t="n">
-        <v>1052353191737.253</v>
+        <v>1090824426406.13</v>
       </c>
       <c r="K35" t="n">
-        <v>106697277586.8798</v>
+        <v>110567116710.5339</v>
       </c>
     </row>
     <row r="36">
@@ -23123,31 +23123,31 @@
         <v>131.824</v>
       </c>
       <c r="C36" t="n">
-        <v>8.946</v>
+        <v>9.069000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>10.652</v>
+        <v>10.63</v>
       </c>
       <c r="E36" t="n">
-        <v>2332.314458370783</v>
+        <v>2359.542454632875</v>
       </c>
       <c r="F36" t="n">
-        <v>23276.66078286807</v>
+        <v>24201.29017712827</v>
       </c>
       <c r="G36" t="n">
-        <v>23276.66078286807</v>
+        <v>24201.29017712827</v>
       </c>
       <c r="H36" t="n">
-        <v>596837455970.9762</v>
+        <v>620545901977.6481</v>
       </c>
       <c r="I36" t="n">
-        <v>596837455970.9762</v>
+        <v>620545901977.6481</v>
       </c>
       <c r="J36" t="n">
-        <v>473292102584.9841</v>
+        <v>492092900268.2749</v>
       </c>
       <c r="K36" t="n">
-        <v>59802934830.02008</v>
+        <v>60501088580.33013</v>
       </c>
     </row>
     <row r="37">
@@ -23156,31 +23156,31 @@
         <v>131.824</v>
       </c>
       <c r="C37" t="n">
-        <v>9.992000000000001</v>
+        <v>9.994</v>
       </c>
       <c r="D37" t="n">
-        <v>10.652</v>
+        <v>10.63</v>
       </c>
       <c r="E37" t="n">
-        <v>2605.342540036494</v>
+        <v>2600.488316916576</v>
       </c>
       <c r="F37" t="n">
-        <v>32445.44487863863</v>
+        <v>32398.11528844508</v>
       </c>
       <c r="G37" t="n">
-        <v>32445.44487863863</v>
+        <v>32398.11528844508</v>
       </c>
       <c r="H37" t="n">
-        <v>831934484067.6572</v>
+        <v>830720904831.9253</v>
       </c>
       <c r="I37" t="n">
-        <v>831934484067.6572</v>
+        <v>830720904831.9253</v>
       </c>
       <c r="J37" t="n">
-        <v>659724045865.6522</v>
+        <v>658761677531.7168</v>
       </c>
       <c r="K37" t="n">
-        <v>66803654872.73064</v>
+        <v>66679187613.24556</v>
       </c>
     </row>
     <row r="38">
@@ -23189,31 +23189,31 @@
         <v>131.825</v>
       </c>
       <c r="C38" t="n">
-        <v>8.946</v>
+        <v>9.069000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>4.051</v>
+        <v>4</v>
       </c>
       <c r="E38" t="n">
-        <v>887.6441743597844</v>
+        <v>888.5303670294603</v>
       </c>
       <c r="F38" t="n">
-        <v>8871.833575393779</v>
+        <v>9126.788564511406</v>
       </c>
       <c r="G38" t="n">
-        <v>8871.833575393779</v>
+        <v>9126.788564511406</v>
       </c>
       <c r="H38" t="n">
-        <v>227482912189.5841</v>
+        <v>234020219602.8565</v>
       </c>
       <c r="I38" t="n">
-        <v>227482912189.5841</v>
+        <v>234020219602.8565</v>
       </c>
       <c r="J38" t="n">
-        <v>180393949366.3402</v>
+        <v>185578034145.0652</v>
       </c>
       <c r="K38" t="n">
-        <v>22760107034.86627</v>
+        <v>22782829923.83232</v>
       </c>
     </row>
     <row r="39">
@@ -23229,28 +23229,28 @@
         <v>6.5</v>
       </c>
       <c r="D39" t="n">
-        <v>4.051</v>
+        <v>4</v>
       </c>
       <c r="E39" t="n">
-        <v>644.8360739687774</v>
+        <v>636.7229193848258</v>
       </c>
       <c r="F39" t="n">
-        <v>3401.298285913998</v>
+        <v>3358.556765916911</v>
       </c>
       <c r="G39" t="n">
-        <v>3401.298285913998</v>
+        <v>3358.556765916911</v>
       </c>
       <c r="H39" t="n">
-        <v>87212776561.8974</v>
+        <v>86116840151.71568</v>
       </c>
       <c r="I39" t="n">
-        <v>87212776561.8974</v>
+        <v>86116840151.71568</v>
       </c>
       <c r="J39" t="n">
-        <v>69159731813.58464</v>
+        <v>68290654240.31053</v>
       </c>
       <c r="K39" t="n">
-        <v>16534258306.89173</v>
+        <v>16326228702.17502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>